<commit_message>
w1 and 2 slides
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/mlm2/website-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/mlm2/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96ED544-7450-3A48-B20C-2936CC1F4F97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D116C97-71B8-5248-A9DE-01A8290E49CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30060" windowHeight="20040" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
+    <workbookView xWindow="19840" yWindow="3880" windowWidth="30060" windowHeight="20040" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>week</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>Prop</t>
+  </si>
+  <si>
+    <t>w1p1</t>
+  </si>
+  <si>
+    <t>w2p1</t>
   </si>
 </sst>
 </file>
@@ -618,7 +624,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F2" sqref="F2"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,6 +693,9 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
@@ -719,7 +728,9 @@
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
initial draft of w3 slides
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/mlm2/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259D0445-E31B-824B-897C-668F479373F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4956D22-2B5E-DC42-B7F0-A3371408A17C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19840" yWindow="3880" windowWidth="30060" windowHeight="20040" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
   <si>
     <t>week</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>homework-1</t>
+  </si>
+  <si>
+    <t>w3p1</t>
   </si>
 </sst>
 </file>
@@ -626,8 +629,8 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I5" sqref="I5"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,7 +766,9 @@
       <c r="C4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>29</v>
       </c>
@@ -798,10 +803,10 @@
         <v>57</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
update w1 lecture link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/mlm2/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4956D22-2B5E-DC42-B7F0-A3371408A17C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544DC1C9-8B0E-1643-BC54-3D3758ED0EE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19840" yWindow="3880" windowWidth="30060" windowHeight="20040" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -129,9 +129,6 @@
     <t>clark</t>
   </si>
   <si>
-    <t>https://youtu.be/W2mCywkvGp4</t>
-  </si>
-  <si>
     <t>https://r4ds.had.co.nz/tidy-data.html; https://r4ds.had.co.nz/relational-data.html</t>
   </si>
   <si>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>w3p1</t>
+  </si>
+  <si>
+    <t>https://youtu.be/F-pvKQ87dcM</t>
   </si>
 </sst>
 </file>
@@ -629,8 +629,8 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <pane xSplit="3" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -700,28 +700,28 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="153" x14ac:dyDescent="0.2">
@@ -735,25 +735,25 @@
         <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -764,10 +764,10 @@
         <v>44302</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>29</v>
@@ -776,10 +776,10 @@
         <v>33</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="85" x14ac:dyDescent="0.2">
@@ -797,25 +797,25 @@
         <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="M5" s="6"/>
     </row>
@@ -831,19 +831,19 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -861,22 +861,22 @@
         <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -894,13 +894,13 @@
         <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -915,19 +915,19 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -946,13 +946,13 @@
       </c>
       <c r="F10" s="3"/>
       <c r="J10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="L10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -967,14 +967,14 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H11" s="3"/>
       <c r="J11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -988,10 +988,10 @@
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
link sw readings to chapter r code
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/mlm2/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBBEE5E-E222-4C4D-A013-D015216ADC77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25F2221-45D7-1F40-BC2B-C95A53919A96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-340" yWindow="460" windowWidth="30060" windowHeight="20040" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
   <si>
     <t>week</t>
   </si>
@@ -162,9 +162,6 @@
     <t>sw; other</t>
   </si>
   <si>
-    <t>; https://www.sds.pub/nonlinearity.html</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ; 12.1-12.4</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>random_intercepts.html#standard-regression</t>
   </si>
   <si>
-    <t>extensions.html#residual-structure; ;https://canvas.uoregon.edu/files/10667756/download?download_frd=1</t>
-  </si>
-  <si>
     <t>extensions.html</t>
   </si>
   <si>
@@ -250,6 +244,15 @@
   </si>
   <si>
     <t>intro.html</t>
+  </si>
+  <si>
+    <t>extensions.html#residual-structure; https://stats.idre.ucla.edu/r/examples/alda/r-applied-longitudinal-data-analysis-ch-7/; https://canvas.uoregon.edu/files/10667756/download?download_frd=1</t>
+  </si>
+  <si>
+    <t>https://stats.idre.ucla.edu/r/examples/alda/r-applied-longitudinal-data-analysis-ch-4/; https://stats.idre.ucla.edu/r/examples/alda/r-applied-longitudinal-data-analysis-ch-5/</t>
+  </si>
+  <si>
+    <t>https://stats.idre.ucla.edu/r/examples/alda/r-applied-longitudinal-data-analysis-ch-6/; https://www.sds.pub/nonlinearity.html</t>
   </si>
 </sst>
 </file>
@@ -631,9 +634,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" workbookViewId="0">
       <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K7" sqref="K7"/>
+      <selection pane="topRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -703,28 +706,28 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="153" x14ac:dyDescent="0.2">
@@ -738,22 +741,22 @@
         <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>34</v>
@@ -767,10 +770,10 @@
         <v>44302</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>29</v>
@@ -779,10 +782,10 @@
         <v>33</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="85" x14ac:dyDescent="0.2">
@@ -796,29 +799,29 @@
         <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -830,22 +833,25 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>35</v>
@@ -869,7 +875,7 @@
         <v>40</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -887,22 +893,22 @@
         <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>41</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>42</v>
@@ -920,7 +926,7 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>16</v>
@@ -945,19 +951,19 @@
       </c>
       <c r="F10" s="3"/>
       <c r="H10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>44</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -972,14 +978,14 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H11" s="3"/>
       <c r="J11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -993,10 +999,10 @@
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
post w3 lecture link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/mlm2/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADF0BAA-14D8-C646-97E5-60F3C9D8D43B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480519C1-8658-4A42-93F2-AC166FB893D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30060" windowHeight="20040" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
   <si>
     <t>week</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>https://youtu.be/dlE_kpoPih0</t>
+  </si>
+  <si>
+    <t>https://youtu.be/0a2lS2tfvXc</t>
   </si>
 </sst>
 </file>
@@ -639,7 +642,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <pane xSplit="3" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q4" sqref="Q4"/>
+      <selection pane="topRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -793,6 +796,9 @@
       <c r="L4" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="M4" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="1">

</xml_diff>

<commit_message>
first full draft of bayes estimation slides
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/mlm2/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4198AF-7562-D847-9016-EAE522DF475F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8144A5-26FA-0044-A88D-28A9965CFDE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6640" yWindow="460" windowWidth="43680" windowHeight="25080" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t>week</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>w6p1</t>
+  </si>
+  <si>
+    <t>w7p1</t>
   </si>
 </sst>
 </file>
@@ -645,7 +648,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D7" sqref="D7"/>
+      <selection pane="topRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,7 +912,9 @@
       <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Post w7 video and a few scripts
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/mlm2/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA90E79-9FB0-884C-95FB-CCE4689CF8B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBDE870-74E0-C048-86E1-01E766277756}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6640" yWindow="460" windowWidth="43680" windowHeight="25080" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="84">
   <si>
     <t>week</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>w8p1</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Au4KTEtt57Y</t>
   </si>
 </sst>
 </file>
@@ -655,9 +658,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -954,6 +957,9 @@
       <c r="L8" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="M8" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="1">

</xml_diff>

<commit_message>
Upload w8 video link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/mlm2/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBDE870-74E0-C048-86E1-01E766277756}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B464CA-820A-E94A-AD3D-7B245A53C104}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6640" yWindow="460" windowWidth="43680" windowHeight="25080" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
   <si>
     <t>week</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>https://youtu.be/Au4KTEtt57Y</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ScT7eD2Mp4k</t>
   </si>
 </sst>
 </file>
@@ -660,7 +663,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
       <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M9" sqref="M9"/>
+      <selection pane="topRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -983,6 +986,9 @@
       <c r="K9" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="M9" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1">

</xml_diff>

<commit_message>
post w9 video link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/mlm2/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596E7F61-8165-E94F-B1E0-70A1D226418C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18177861-F911-A44F-9576-5BD8DF7CD6F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6640" yWindow="460" windowWidth="43680" windowHeight="25080" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="87">
   <si>
     <t>week</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>w9p1</t>
+  </si>
+  <si>
+    <t>https://youtu.be/YaLS2eqoUXs</t>
   </si>
 </sst>
 </file>
@@ -664,9 +667,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1025,6 +1028,9 @@
       <c r="L10" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="M10" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="1">

</xml_diff>

<commit_message>
post w10 video link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/mlm2/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B245BA30-0227-4944-A24B-EE8AEC5229FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B53AAD-F5DD-784A-8091-D6ECDE0D83F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6640" yWindow="460" windowWidth="43680" windowHeight="25080" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
   <si>
     <t>week</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>We fit several multilevel binomial logistic regression models using Bayesian estimation. We walk through two full examples, including data exploration to analysis to interpretation. This includes post-hoc comparisons computed using samples from the posterior distribution.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ezPNfJqKT04</t>
   </si>
 </sst>
 </file>
@@ -671,8 +674,8 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E14" sqref="E14"/>
+      <pane xSplit="3" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1058,6 +1061,9 @@
       <c r="K11" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="M11" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">

</xml_diff>